<commit_message>
More work on the turboprop database model.
</commit_message>
<xml_diff>
--- a/DOCS/TurboporpEngineModel/PW2750.xlsx
+++ b/DOCS/TurboporpEngineModel/PW2750.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PW2750 TAKE-OFF" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -286,12 +286,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -386,7 +386,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -502,7 +502,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A9A6-4E6D-A87F-B3FF630BAB34}"/>
@@ -623,7 +623,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A9A6-4E6D-A87F-B3FF630BAB34}"/>
@@ -744,7 +744,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-A9A6-4E6D-A87F-B3FF630BAB34}"/>
@@ -865,7 +865,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A9A6-4E6D-A87F-B3FF630BAB34}"/>
@@ -1271,7 +1271,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1387,7 +1387,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2F68-4922-BDEE-D112FC729F40}"/>
@@ -1508,7 +1508,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2F68-4922-BDEE-D112FC729F40}"/>
@@ -1629,7 +1629,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2F68-4922-BDEE-D112FC729F40}"/>
@@ -1750,7 +1750,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-2F68-4922-BDEE-D112FC729F40}"/>
@@ -1871,7 +1871,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-2F68-4922-BDEE-D112FC729F40}"/>
@@ -1992,7 +1992,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-2F68-4922-BDEE-D112FC729F40}"/>
@@ -2115,7 +2115,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-2F68-4922-BDEE-D112FC729F40}"/>
@@ -2521,7 +2521,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2637,7 +2637,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1562-4A7C-8F7F-C5EF0135E2A2}"/>
@@ -2758,7 +2758,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1562-4A7C-8F7F-C5EF0135E2A2}"/>
@@ -2879,7 +2879,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1562-4A7C-8F7F-C5EF0135E2A2}"/>
@@ -3000,7 +3000,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-1562-4A7C-8F7F-C5EF0135E2A2}"/>
@@ -3406,7 +3406,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -3522,7 +3522,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5E75-4C1B-93A5-4842315EBA46}"/>
@@ -3643,7 +3643,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5E75-4C1B-93A5-4842315EBA46}"/>
@@ -3764,7 +3764,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5E75-4C1B-93A5-4842315EBA46}"/>
@@ -3885,7 +3885,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-5E75-4C1B-93A5-4842315EBA46}"/>
@@ -4006,7 +4006,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-5E75-4C1B-93A5-4842315EBA46}"/>
@@ -4127,7 +4127,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-5E75-4C1B-93A5-4842315EBA46}"/>
@@ -4250,7 +4250,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-5E75-4C1B-93A5-4842315EBA46}"/>
@@ -4654,9 +4654,19 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17314429550821198"/>
+          <c:y val="0.12215112736136502"/>
+          <c:w val="0.783112781888886"/>
+          <c:h val="0.63515069071576291"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -4772,7 +4782,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3A8E-4F74-B257-44AFC39F54FC}"/>
@@ -4893,7 +4903,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3A8E-4F74-B257-44AFC39F54FC}"/>
@@ -5014,7 +5024,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3A8E-4F74-B257-44AFC39F54FC}"/>
@@ -5135,7 +5145,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-3A8E-4F74-B257-44AFC39F54FC}"/>
@@ -5256,7 +5266,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-3A8E-4F74-B257-44AFC39F54FC}"/>
@@ -5377,7 +5387,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-3A8E-4F74-B257-44AFC39F54FC}"/>
@@ -5500,7 +5510,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-3A8E-4F74-B257-44AFC39F54FC}"/>
@@ -5906,7 +5916,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -6022,7 +6032,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C11A-40B6-8EDB-AF6CE9A5B7B1}"/>
@@ -6143,7 +6153,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C11A-40B6-8EDB-AF6CE9A5B7B1}"/>
@@ -6264,7 +6274,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C11A-40B6-8EDB-AF6CE9A5B7B1}"/>
@@ -6385,7 +6395,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-C11A-40B6-8EDB-AF6CE9A5B7B1}"/>
@@ -6506,7 +6516,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-C11A-40B6-8EDB-AF6CE9A5B7B1}"/>
@@ -6627,7 +6637,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-C11A-40B6-8EDB-AF6CE9A5B7B1}"/>
@@ -6750,7 +6760,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-C11A-40B6-8EDB-AF6CE9A5B7B1}"/>
@@ -7156,7 +7166,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -7272,7 +7282,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DB8D-4695-A8DF-1DAAEFC27DA7}"/>
@@ -7393,7 +7403,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DB8D-4695-A8DF-1DAAEFC27DA7}"/>
@@ -7514,7 +7524,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-DB8D-4695-A8DF-1DAAEFC27DA7}"/>
@@ -7635,7 +7645,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-DB8D-4695-A8DF-1DAAEFC27DA7}"/>
@@ -7756,7 +7766,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-DB8D-4695-A8DF-1DAAEFC27DA7}"/>
@@ -7877,7 +7887,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-DB8D-4695-A8DF-1DAAEFC27DA7}"/>
@@ -8000,7 +8010,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-DB8D-4695-A8DF-1DAAEFC27DA7}"/>
@@ -8406,7 +8416,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -8522,7 +8532,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CA83-4EC4-A159-DA7AEC3DC587}"/>
@@ -8643,7 +8653,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CA83-4EC4-A159-DA7AEC3DC587}"/>
@@ -8764,7 +8774,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-CA83-4EC4-A159-DA7AEC3DC587}"/>
@@ -8885,7 +8895,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-CA83-4EC4-A159-DA7AEC3DC587}"/>
@@ -9006,7 +9016,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-CA83-4EC4-A159-DA7AEC3DC587}"/>
@@ -9127,7 +9137,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-CA83-4EC4-A159-DA7AEC3DC587}"/>
@@ -9250,7 +9260,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-CA83-4EC4-A159-DA7AEC3DC587}"/>
@@ -9656,7 +9666,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -9772,7 +9782,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EAFE-445E-A074-F8669CC73092}"/>
@@ -9893,7 +9903,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EAFE-445E-A074-F8669CC73092}"/>
@@ -10014,7 +10024,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-EAFE-445E-A074-F8669CC73092}"/>
@@ -10135,7 +10145,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-EAFE-445E-A074-F8669CC73092}"/>
@@ -10256,7 +10266,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-EAFE-445E-A074-F8669CC73092}"/>
@@ -10377,7 +10387,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-EAFE-445E-A074-F8669CC73092}"/>
@@ -10500,7 +10510,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-EAFE-445E-A074-F8669CC73092}"/>
@@ -10906,7 +10916,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -11022,7 +11032,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-88CB-492E-8626-1DE791C6E9FF}"/>
@@ -11143,7 +11153,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-88CB-492E-8626-1DE791C6E9FF}"/>
@@ -11264,7 +11274,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-88CB-492E-8626-1DE791C6E9FF}"/>
@@ -11385,7 +11395,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-88CB-492E-8626-1DE791C6E9FF}"/>
@@ -11506,7 +11516,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-88CB-492E-8626-1DE791C6E9FF}"/>
@@ -11627,7 +11637,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-88CB-492E-8626-1DE791C6E9FF}"/>
@@ -11750,7 +11760,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-88CB-492E-8626-1DE791C6E9FF}"/>
@@ -18342,7 +18352,7 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -25664,8 +25674,8 @@
   <sheetPr codeName="Foglio5"/>
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
More work on saveAircraftToXML. More tests on ACPerformanceManager.
</commit_message>
<xml_diff>
--- a/DOCS/TurboporpEngineModel/PW2750.xlsx
+++ b/DOCS/TurboporpEngineModel/PW2750.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <workbookPr codeName="Questa_cartella_di_lavoro"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vittorio\ADOPT_PROJECT\jpad\DOCS\TurboporpEngineModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\JPAD\jpad\DOCS\TurboporpEngineModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="PW2750 TAKE-OFF" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="PW2750 CRUISE" sheetId="4" r:id="rId4"/>
     <sheet name="PW2750 IDLE" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="7">
   <si>
     <t>Altitude</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>T/T0</t>
+  </si>
+  <si>
+    <t>MEAN</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -292,6 +295,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -18350,20 +18354,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Foglio1"/>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -18383,7 +18387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -18405,7 +18409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>0</v>
       </c>
@@ -18427,7 +18431,7 @@
         <v>0.94460539136083144</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>0</v>
       </c>
@@ -18449,7 +18453,7 @@
         <v>0.86360506658005853</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>0</v>
       </c>
@@ -18471,7 +18475,7 @@
         <v>0.74854173432932769</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>0</v>
       </c>
@@ -18493,7 +18497,7 @@
         <v>0.63551802533290025</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>0</v>
       </c>
@@ -18515,7 +18519,7 @@
         <v>0.54556674244884706</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>0</v>
       </c>
@@ -18537,7 +18541,7 @@
         <v>0.47225722637219875</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>0</v>
       </c>
@@ -18559,7 +18563,7 @@
         <v>0.40858720363754464</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>0</v>
       </c>
@@ -18581,7 +18585,7 @@
         <v>0.35572588502760633</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>0</v>
       </c>
@@ -18603,7 +18607,7 @@
         <v>0.30373497888924977</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>0</v>
       </c>
@@ -18625,7 +18629,7 @@
         <v>0.25234166937317309</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>0</v>
       </c>
@@ -18647,7 +18651,7 @@
         <v>0.20093536862617734</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>0</v>
       </c>
@@ -18669,7 +18673,7 @@
         <v>0.15216628775576485</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>5000</v>
       </c>
@@ -18691,7 +18695,7 @@
         <v>0.8799610263072426</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>5000</v>
       </c>
@@ -18713,7 +18717,7 @@
         <v>0.86064306593049689</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>5000</v>
       </c>
@@ -18735,7 +18739,7 @@
         <v>0.81658980188372843</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5000</v>
       </c>
@@ -18757,7 +18761,7 @@
         <v>0.7269243260798961</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>5000</v>
       </c>
@@ -18779,7 +18783,7 @@
         <v>0.62997076973043198</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>5000</v>
       </c>
@@ -18801,7 +18805,7 @@
         <v>0.54615134784020791</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>5000</v>
       </c>
@@ -18823,7 +18827,7 @@
         <v>0.47605066580058464</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>5000</v>
       </c>
@@ -18845,7 +18849,7 @@
         <v>0.41588827541409551</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>5000</v>
       </c>
@@ -18867,7 +18871,7 @@
         <v>0.36594998376096138</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>5000</v>
       </c>
@@ -18889,7 +18893,7 @@
         <v>0.31892172783371225</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>5000</v>
       </c>
@@ -18911,7 +18915,7 @@
         <v>0.27219227021760312</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>5000</v>
       </c>
@@ -18933,7 +18937,7 @@
         <v>0.22576161091263397</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>5000</v>
       </c>
@@ -18955,7 +18959,7 @@
         <v>0.17990256576810651</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>10000</v>
       </c>
@@ -18977,7 +18981,7 @@
         <v>0.75905164014290361</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>10000</v>
       </c>
@@ -18999,7 +19003,7 @@
         <v>0.7491912958752841</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>10000</v>
       </c>
@@ -19021,7 +19025,7 @@
         <v>0.72430009743423196</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>10000</v>
       </c>
@@ -19042,8 +19046,12 @@
         <f t="shared" si="2"/>
         <v>0.65215979214030528</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <f>2750/D2</f>
+        <v>0.35725885027606363</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>10000</v>
       </c>
@@ -19065,7 +19073,7 @@
         <v>0.56834037025008122</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>10000</v>
       </c>
@@ -19087,7 +19095,7 @@
         <v>0.49912309191295873</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>10000</v>
       </c>
@@ -19109,7 +19117,7 @@
         <v>0.44713218577460218</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>10000</v>
       </c>
@@ -19131,7 +19139,7 @@
         <v>0.40507957128937966</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>10000</v>
       </c>
@@ -19153,7 +19161,7 @@
         <v>0.37149723936342965</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>10000</v>
       </c>
@@ -19175,7 +19183,7 @@
         <v>0.33061383566092889</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>10000</v>
       </c>
@@ -19197,7 +19205,7 @@
         <v>0.28796362455342644</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>10000</v>
       </c>
@@ -19219,7 +19227,7 @@
         <v>0.24708022085092562</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>10000</v>
       </c>
@@ -19241,7 +19249,7 @@
         <v>0.20619681714842483</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>15000</v>
       </c>
@@ -19263,7 +19271,7 @@
         <v>0.64719714192919786</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>15000</v>
       </c>
@@ -19285,7 +19293,7 @@
         <v>0.63898668398830794</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>15000</v>
       </c>
@@ -19307,7 +19315,7 @@
         <v>0.61827866190321534</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>15000</v>
       </c>
@@ -19329,7 +19337,7 @@
         <v>0.55841506982786615</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>15000</v>
       </c>
@@ -19351,7 +19359,7 @@
         <v>0.48889899317960378</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>15000</v>
       </c>
@@ -19373,7 +19381,7 @@
         <v>0.42552776875608966</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>15000</v>
       </c>
@@ -19395,7 +19403,7 @@
         <v>0.38200714517700551</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>15000</v>
       </c>
@@ -19417,7 +19425,7 @@
         <v>0.34725560246833387</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>15000</v>
       </c>
@@ -19439,7 +19447,7 @@
         <v>0.31922052614485219</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>15000</v>
       </c>
@@ -19461,7 +19469,7 @@
         <v>0.29556349464111725</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>15000</v>
       </c>
@@ -19483,7 +19491,7 @@
         <v>0.27307567392010396</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>15000</v>
       </c>
@@ -19505,7 +19513,7 @@
         <v>0.25292627476453394</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>15000</v>
       </c>
@@ -19543,14 +19551,14 @@
       <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -19570,7 +19578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -19592,7 +19600,7 @@
         <v>1.0014550178629424</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>0</v>
       </c>
@@ -19614,7 +19622,7 @@
         <v>0.94778824293601827</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>0</v>
       </c>
@@ -19636,7 +19644,7 @@
         <v>0.86799610263072424</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>0</v>
       </c>
@@ -19658,7 +19666,7 @@
         <v>0.75320558622929523</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>0</v>
       </c>
@@ -19680,7 +19688,7 @@
         <v>0.64018187723286779</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>0</v>
       </c>
@@ -19702,7 +19710,7 @@
         <v>0.54964598895745365</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>0</v>
       </c>
@@ -19724,7 +19732,7 @@
         <v>0.47576485872036373</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>0</v>
       </c>
@@ -19746,7 +19754,7 @@
         <v>0.41209483598570962</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>0</v>
       </c>
@@ -19768,7 +19776,7 @@
         <v>0.35864891198441051</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>0</v>
       </c>
@@ -19790,7 +19798,7 @@
         <v>0.3066580058460539</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>0</v>
       </c>
@@ -19812,7 +19820,7 @@
         <v>0.25496589801883729</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>0</v>
       </c>
@@ -19834,7 +19842,7 @@
         <v>0.20355959727184153</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>0</v>
       </c>
@@ -19856,7 +19864,7 @@
         <v>0.15449171809028905</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>5000</v>
       </c>
@@ -19878,7 +19886,7 @@
         <v>0.88054563169860345</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>5000</v>
       </c>
@@ -19900,7 +19908,7 @@
         <v>0.86225397856446895</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>5000</v>
       </c>
@@ -19922,7 +19930,7 @@
         <v>0.82009743423189341</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5000</v>
       </c>
@@ -19944,7 +19952,7 @@
         <v>0.73101656381942193</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>5000</v>
       </c>
@@ -19966,7 +19974,7 @@
         <v>0.63405001623903867</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>5000</v>
       </c>
@@ -19988,7 +19996,7 @@
         <v>0.55023059434881449</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>5000</v>
       </c>
@@ -20010,7 +20018,7 @@
         <v>0.47955829814874962</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>5000</v>
       </c>
@@ -20032,7 +20040,7 @@
         <v>0.4190971094511205</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>5000</v>
       </c>
@@ -20054,7 +20062,7 @@
         <v>0.36887301071776551</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>5000</v>
       </c>
@@ -20076,7 +20084,7 @@
         <v>0.32184475479051644</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>5000</v>
       </c>
@@ -20098,7 +20106,7 @@
         <v>0.27482949009418645</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>5000</v>
       </c>
@@ -20120,7 +20128,7 @@
         <v>0.22838583955829814</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>5000</v>
       </c>
@@ -20142,7 +20150,7 @@
         <v>0.18253978564468981</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>10000</v>
       </c>
@@ -20164,7 +20172,7 @@
         <v>0.76431308866515102</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>10000</v>
       </c>
@@ -20186,7 +20194,7 @@
         <v>0.76378044819746671</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>10000</v>
       </c>
@@ -20208,7 +20216,7 @@
         <v>0.76197466709970774</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>10000</v>
       </c>
@@ -20230,7 +20238,7 @@
         <v>0.70181227671321855</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>10000</v>
       </c>
@@ -20252,7 +20260,7 @@
         <v>0.61799285482299449</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>10000</v>
       </c>
@@ -20274,7 +20282,7 @@
         <v>0.54643715492042866</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>10000</v>
       </c>
@@ -20296,7 +20304,7 @@
         <v>0.48072750893147126</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>10000</v>
       </c>
@@ -20318,7 +20326,7 @@
         <v>0.42464436505358882</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>10000</v>
       </c>
@@ -20340,7 +20348,7 @@
         <v>0.37645988957453719</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>10000</v>
       </c>
@@ -20362,7 +20370,7 @@
         <v>0.33352387138681394</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>10000</v>
       </c>
@@ -20384,7 +20392,7 @@
         <v>0.29088665151023058</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>10000</v>
       </c>
@@ -20406,7 +20414,7 @@
         <v>0.25000324780772981</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>10000</v>
       </c>
@@ -20428,7 +20436,7 @@
         <v>0.208821045794089</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>15000</v>
       </c>
@@ -20450,7 +20458,7 @@
         <v>0.65245859045144527</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>15000</v>
       </c>
@@ -20472,7 +20480,7 @@
         <v>0.65347190646313746</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>15000</v>
       </c>
@@ -20494,7 +20502,7 @@
         <v>0.65361481000324784</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>15000</v>
       </c>
@@ -20516,7 +20524,7 @@
         <v>0.60426112374147456</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>15000</v>
       </c>
@@ -20538,7 +20546,7 @@
         <v>0.53475803832413127</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>15000</v>
       </c>
@@ -20560,7 +20568,7 @@
         <v>0.46962000649561547</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>15000</v>
       </c>
@@ -20582,7 +20590,7 @@
         <v>0.42347515427086713</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>15000</v>
       </c>
@@ -20604,7 +20612,7 @@
         <v>0.38580058460539135</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>15000</v>
       </c>
@@ -20626,7 +20634,7 @@
         <v>0.35572588502760633</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>15000</v>
       </c>
@@ -20648,7 +20656,7 @@
         <v>0.33002923026956804</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>15000</v>
       </c>
@@ -20670,7 +20678,7 @@
         <v>0.30461838259175061</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>15000</v>
       </c>
@@ -20692,7 +20700,7 @@
         <v>0.26869762910035727</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>15000</v>
       </c>
@@ -20714,7 +20722,7 @@
         <v>0.23247807729782397</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>20000</v>
       </c>
@@ -20736,7 +20744,7 @@
         <v>0.55373822669697947</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>20000</v>
       </c>
@@ -20758,7 +20766,7 @@
         <v>0.55680415719389409</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>20000</v>
       </c>
@@ -20780,7 +20788,7 @@
         <v>0.55724585904514445</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>20000</v>
       </c>
@@ -20802,7 +20810,7 @@
         <v>0.51840207859694709</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>20000</v>
       </c>
@@ -20824,7 +20832,7 @@
         <v>0.46114972393634296</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>20000</v>
       </c>
@@ -20846,7 +20854,7 @@
         <v>0.4059629749918805</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>20000</v>
       </c>
@@ -20868,7 +20876,7 @@
         <v>0.36127314063007471</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>20000</v>
       </c>
@@ -20890,7 +20898,7 @@
         <v>0.32944462487820725</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>20000</v>
       </c>
@@ -20912,7 +20920,7 @@
         <v>0.30431958428061057</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>20000</v>
       </c>
@@ -20934,7 +20942,7 @@
         <v>0.28271516726209805</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>20000</v>
       </c>
@@ -20956,7 +20964,7 @@
         <v>0.26255277687560896</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>20000</v>
       </c>
@@ -20978,7 +20986,7 @@
         <v>0.24562520298798313</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <v>20000</v>
       </c>
@@ -21000,7 +21008,7 @@
         <v>0.23072426112374148</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>25000</v>
       </c>
@@ -21022,7 +21030,7 @@
         <v>0.46670997076973042</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>25000</v>
       </c>
@@ -21044,7 +21052,7 @@
         <v>0.4710490418967197</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>25000</v>
       </c>
@@ -21066,7 +21074,7 @@
         <v>0.4716726209808379</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>25000</v>
       </c>
@@ -21088,7 +21096,7 @@
         <v>0.44188372848327379</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>25000</v>
       </c>
@@ -21110,7 +21118,7 @@
         <v>0.3957388762585255</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>25000</v>
       </c>
@@ -21132,7 +21140,7 @@
         <v>0.34987983111399801</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>25000</v>
       </c>
@@ -21154,7 +21162,7 @@
         <v>0.3081130237089964</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>25000</v>
       </c>
@@ -21176,7 +21184,7 @@
         <v>0.28037674569665472</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>25000</v>
       </c>
@@ -21198,7 +21206,7 @@
         <v>0.25964274114972391</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>25000</v>
       </c>
@@ -21220,7 +21228,7 @@
         <v>0.24211757063981812</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>25000</v>
       </c>
@@ -21242,7 +21250,7 @@
         <v>0.22429360181877234</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>25000</v>
       </c>
@@ -21264,7 +21272,7 @@
         <v>0.20969145826567065</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="9">
         <v>25000</v>
       </c>
@@ -21286,7 +21294,7 @@
         <v>0.19801234166937318</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>30000</v>
       </c>
@@ -21308,7 +21316,7 @@
         <v>0.39019162065605717</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>30000</v>
       </c>
@@ -21330,7 +21338,7 @@
         <v>0.39503734978889254</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>30000</v>
       </c>
@@ -21352,7 +21360,7 @@
         <v>0.3957388762585255</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>30000</v>
       </c>
@@ -21374,7 +21382,7 @@
         <v>0.37295225722637221</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>30000</v>
       </c>
@@ -21396,7 +21404,7 @@
         <v>0.33586229295225722</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>30000</v>
       </c>
@@ -21418,7 +21426,7 @@
         <v>0.2976031178954206</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>30000</v>
       </c>
@@ -21440,7 +21448,7 @@
         <v>0.26285157518674895</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>30000</v>
       </c>
@@ -21462,7 +21470,7 @@
         <v>0.23393309516076649</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>30000</v>
       </c>
@@ -21484,7 +21492,7 @@
         <v>0.21729132835336146</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>30000</v>
       </c>
@@ -21506,7 +21514,7 @@
         <v>0.20414420266320235</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>30000</v>
       </c>
@@ -21528,7 +21536,7 @@
         <v>0.18925625202987983</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>30000</v>
       </c>
@@ -21550,7 +21558,7 @@
         <v>0.1775641442026632</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="9">
         <v>30000</v>
       </c>
@@ -21588,14 +21596,14 @@
       <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -21615,7 +21623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -21637,7 +21645,7 @@
         <v>0.69856446898343616</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>0</v>
       </c>
@@ -21659,7 +21667,7 @@
         <v>0.70699577784995138</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>0</v>
       </c>
@@ -21681,7 +21689,7 @@
         <v>0.70820396232543026</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>0</v>
       </c>
@@ -21703,7 +21711,7 @@
         <v>0.64424813251055546</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>0</v>
       </c>
@@ -21725,7 +21733,7 @@
         <v>0.55750568366352704</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>0</v>
       </c>
@@ -21747,7 +21755,7 @@
         <v>0.48070152646963299</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>0</v>
       </c>
@@ -21769,7 +21777,7 @@
         <v>0.41557648587203638</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>0</v>
       </c>
@@ -21791,7 +21799,7 @@
         <v>0.36126014939915557</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>0</v>
       </c>
@@ -21813,7 +21821,7 @@
         <v>0.31598570964598899</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>0</v>
       </c>
@@ -21835,7 +21843,7 @@
         <v>0.27568691133484896</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>0</v>
       </c>
@@ -21857,7 +21865,7 @@
         <v>0.23567392010392985</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>0</v>
       </c>
@@ -21879,7 +21887,7 @@
         <v>0.19303670022734656</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>0</v>
       </c>
@@ -21901,7 +21909,7 @@
         <v>0.1515686911334849</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>5000</v>
       </c>
@@ -21923,7 +21931,7 @@
         <v>0.60131211432283216</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>5000</v>
       </c>
@@ -21945,7 +21953,7 @@
         <v>0.62962000649561545</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>5000</v>
       </c>
@@ -21967,7 +21975,7 @@
         <v>0.63460863916856114</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5000</v>
       </c>
@@ -21989,7 +21997,7 @@
         <v>0.60627476453393958</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>5000</v>
       </c>
@@ -22011,7 +22019,7 @@
         <v>0.5356024683338747</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>5000</v>
       </c>
@@ -22033,7 +22041,7 @@
         <v>0.47369925300422216</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>5000</v>
       </c>
@@ -22055,7 +22063,7 @@
         <v>0.41849951282884057</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>5000</v>
       </c>
@@ -22077,7 +22085,7 @@
         <v>0.36650860669048391</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>5000</v>
       </c>
@@ -22099,7 +22107,7 @@
         <v>0.32300097434231895</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>5000</v>
       </c>
@@ -22121,7 +22129,7 @@
         <v>0.28561221175706397</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>5000</v>
       </c>
@@ -22143,7 +22151,7 @@
         <v>0.24999025657681065</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>5000</v>
       </c>
@@ -22165,7 +22173,7 @@
         <v>0.21144527443975317</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>5000</v>
       </c>
@@ -22187,7 +22195,7 @@
         <v>0.17405651185449822</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>10000</v>
       </c>
@@ -22209,7 +22217,7 @@
         <v>0.51486846378694384</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>10000</v>
       </c>
@@ -22231,7 +22239,7 @@
         <v>0.54155245209483605</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>10000</v>
       </c>
@@ -22253,7 +22261,7 @@
         <v>0.54903540110425464</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>10000</v>
       </c>
@@ -22275,7 +22283,7 @@
         <v>0.53414745047093215</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>10000</v>
       </c>
@@ -22297,7 +22305,7 @@
         <v>0.47924650860669049</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>10000</v>
       </c>
@@ -22319,7 +22327,7 @@
         <v>0.42346216303994805</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>10000</v>
       </c>
@@ -22341,7 +22349,7 @@
         <v>0.37761610912633969</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>10000</v>
       </c>
@@ -22363,7 +22371,7 @@
         <v>0.33964274114972393</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>10000</v>
       </c>
@@ -22385,7 +22393,7 @@
         <v>0.30868463786943812</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>10000</v>
       </c>
@@ -22407,7 +22415,7 @@
         <v>0.28328678142253977</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>10000</v>
       </c>
@@ -22429,7 +22437,7 @@
         <v>0.26108476778174733</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>10000</v>
       </c>
@@ -22451,7 +22459,7 @@
         <v>0.22837284832737903</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>10000</v>
       </c>
@@ -22473,7 +22481,7 @@
         <v>0.19595972718415072</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>15000</v>
       </c>
@@ -22495,7 +22503,7 @@
         <v>0.43864891198441053</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>15000</v>
       </c>
@@ -22517,7 +22525,7 @@
         <v>0.46347515427086716</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>15000</v>
       </c>
@@ -22539,7 +22547,7 @@
         <v>0.47253004222150052</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>15000</v>
       </c>
@@ -22561,7 +22569,7 @@
         <v>0.46755440077947386</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>15000</v>
       </c>
@@ -22583,7 +22591,7 @@
         <v>0.42521597921403054</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>15000</v>
       </c>
@@ -22605,7 +22613,7 @@
         <v>0.37644689834361805</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>15000</v>
       </c>
@@ -22627,7 +22635,7 @@
         <v>0.33935693406950307</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>15000</v>
       </c>
@@ -22649,7 +22657,7 @@
         <v>0.30781422539785647</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>15000</v>
       </c>
@@ -22671,7 +22679,7 @@
         <v>0.28094835985709643</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>15000</v>
       </c>
@@ -22693,7 +22701,7 @@
         <v>0.25874634621630399</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>15000</v>
       </c>
@@ -22715,7 +22723,7 @@
         <v>0.23918155245209483</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>15000</v>
       </c>
@@ -22737,7 +22745,7 @@
         <v>0.2193179603767457</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>15000</v>
       </c>
@@ -22759,7 +22767,7 @@
         <v>0.20033777200389735</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>20000</v>
       </c>
@@ -22781,7 +22789,7 @@
         <v>0.37206885352387137</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>20000</v>
       </c>
@@ -22803,7 +22811,7 @@
         <v>0.39253004222150051</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>20000</v>
       </c>
@@ -22825,7 +22833,7 @@
         <v>0.40068853523871389</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>20000</v>
       </c>
@@ -22847,7 +22855,7 @@
         <v>0.39951932445599225</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>20000</v>
       </c>
@@ -22869,7 +22877,7 @@
         <v>0.36476778174732061</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>20000</v>
       </c>
@@ -22891,7 +22899,7 @@
         <v>0.32445599220526145</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>20000</v>
       </c>
@@ -22913,7 +22921,7 @@
         <v>0.28911984410522895</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>20000</v>
       </c>
@@ -22935,7 +22943,7 @@
         <v>0.26370899642741152</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>20000</v>
       </c>
@@ -22957,7 +22965,7 @@
         <v>0.24297499188048066</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>20000</v>
       </c>
@@ -22979,7 +22987,7 @@
         <v>0.22604741799285483</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>20000</v>
       </c>
@@ -23001,7 +23009,7 @@
         <v>0.21201688860019488</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>20000</v>
       </c>
@@ -23023,7 +23031,7 @@
         <v>0.19829814874959403</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <v>20000</v>
       </c>
@@ -23045,7 +23053,7 @@
         <v>0.18486521597921404</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>25000</v>
       </c>
@@ -23067,7 +23075,7 @@
         <v>0.31394608639168559</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>25000</v>
       </c>
@@ -23089,7 +23097,7 @@
         <v>0.33052289704449495</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>25000</v>
       </c>
@@ -23111,7 +23119,7 @@
         <v>0.33760311789542058</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>25000</v>
       </c>
@@ -23133,7 +23141,7 @@
         <v>0.33788892497564144</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>25000</v>
       </c>
@@ -23155,7 +23163,7 @@
         <v>0.30956804157193896</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>25000</v>
       </c>
@@ -23177,7 +23185,7 @@
         <v>0.27627151672620981</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>25000</v>
       </c>
@@ -23199,7 +23207,7 @@
         <v>0.24385839558298147</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>25000</v>
       </c>
@@ -23221,7 +23229,7 @@
         <v>0.221955180253329</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>25000</v>
       </c>
@@ -23243,7 +23251,7 @@
         <v>0.20471581682364404</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>25000</v>
       </c>
@@ -23265,7 +23273,7 @@
         <v>0.19099707697304319</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>25000</v>
       </c>
@@ -23287,7 +23295,7 @@
         <v>0.17960376745696655</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>25000</v>
       </c>
@@ -23309,7 +23317,7 @@
         <v>0.16937966872361154</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="9">
         <v>25000</v>
       </c>
@@ -23331,7 +23339,7 @@
         <v>0.15858395582981488</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>30000</v>
       </c>
@@ -23353,7 +23361,7 @@
         <v>0.25582331925949986</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>30000</v>
       </c>
@@ -23375,7 +23383,7 @@
         <v>0.26851575186748944</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>30000</v>
       </c>
@@ -23397,7 +23405,7 @@
         <v>0.27451770055212732</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>30000</v>
       </c>
@@ -23419,7 +23427,7 @@
         <v>0.27627151672620981</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>30000</v>
       </c>
@@ -23441,7 +23449,7 @@
         <v>0.25436830139655731</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>30000</v>
       </c>
@@ -23463,7 +23471,7 @@
         <v>0.22808704124715817</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>30000</v>
       </c>
@@ -23485,7 +23493,7 @@
         <v>0.19858395582981486</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>30000</v>
       </c>
@@ -23507,7 +23515,7 @@
         <v>0.18018837284832737</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>30000</v>
       </c>
@@ -23529,7 +23537,7 @@
         <v>0.16646963299772655</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>30000</v>
       </c>
@@ -23551,7 +23559,7 @@
         <v>0.15594673595323158</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>30000</v>
       </c>
@@ -23573,7 +23581,7 @@
         <v>0.14719064631373824</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>30000</v>
       </c>
@@ -23595,7 +23603,7 @@
         <v>0.14047417992854822</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="9">
         <v>30000</v>
       </c>
@@ -23627,20 +23635,20 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Foglio4"/>
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F67" sqref="F67:F79"/>
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -23660,7 +23668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -23682,7 +23690,7 @@
         <v>0.69681065280935361</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>0</v>
       </c>
@@ -23704,7 +23712,7 @@
         <v>0.70064306593049686</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>0</v>
       </c>
@@ -23726,7 +23734,7 @@
         <v>0.7011886976291003</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>0</v>
       </c>
@@ -23748,7 +23756,7 @@
         <v>0.63227021760311786</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>0</v>
       </c>
@@ -23770,7 +23778,7 @@
         <v>0.54495615459564795</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>0</v>
       </c>
@@ -23792,7 +23800,7 @@
         <v>0.4687236115621955</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>0</v>
       </c>
@@ -23814,7 +23822,7 @@
         <v>0.40476778174732053</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>0</v>
       </c>
@@ -23836,7 +23844,7 @@
         <v>0.35132185774602148</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>0</v>
       </c>
@@ -23858,7 +23866,7 @@
         <v>0.30693082169535563</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>0</v>
       </c>
@@ -23880,7 +23888,7 @@
         <v>0.2672166287755765</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>0</v>
       </c>
@@ -23902,7 +23910,7 @@
         <v>0.22750243585579735</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>0</v>
       </c>
@@ -23924,7 +23932,7 @@
         <v>0.18573562845079572</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>0</v>
       </c>
@@ -23946,7 +23954,7 @@
         <v>0.14456641766807404</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>5000</v>
       </c>
@@ -23968,7 +23976,7 @@
         <v>0.60248444300097437</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>5000</v>
       </c>
@@ -23990,7 +23998,7 @@
         <v>0.62676050665800576</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>5000</v>
       </c>
@@ -24012,7 +24020,7 @@
         <v>0.63022851575186756</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5000</v>
       </c>
@@ -24034,7 +24042,7 @@
         <v>0.59547541409548554</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>5000</v>
       </c>
@@ -24056,7 +24064,7 @@
         <v>0.52217265345891528</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>5000</v>
       </c>
@@ -24078,7 +24086,7 @@
         <v>0.45996752192270218</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>5000</v>
       </c>
@@ -24100,7 +24108,7 @@
         <v>0.40798389087366027</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>5000</v>
       </c>
@@ -24122,7 +24130,7 @@
         <v>0.3568763884378045</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>5000</v>
       </c>
@@ -24144,7 +24152,7 @@
         <v>0.31394608639168559</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>5000</v>
       </c>
@@ -24166,7 +24174,7 @@
         <v>0.2771486846378694</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>5000</v>
       </c>
@@ -24188,7 +24196,7 @@
         <v>0.24181149723936343</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>5000</v>
       </c>
@@ -24210,7 +24218,7 @@
         <v>0.20326183825917504</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>5000</v>
       </c>
@@ -24232,7 +24240,7 @@
         <v>0.1650042221500487</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>10000</v>
       </c>
@@ -24254,7 +24262,7 @@
         <v>0.51633647288080542</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>10000</v>
       </c>
@@ -24276,7 +24284,7 @@
         <v>0.54026632023384213</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>10000</v>
       </c>
@@ -24298,7 +24306,7 @@
         <v>0.5452419616758688</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>10000</v>
       </c>
@@ -24320,7 +24328,7 @@
         <v>0.52450795712893794</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>10000</v>
       </c>
@@ -24342,7 +24350,7 @@
         <v>0.46668398830789221</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>10000</v>
       </c>
@@ -24364,7 +24372,7 @@
         <v>0.41061383566092885</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>10000</v>
       </c>
@@ -24386,7 +24394,7 @@
         <v>0.36650860669048391</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>10000</v>
       </c>
@@ -24408,7 +24416,7 @@
         <v>0.32941864241636892</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>10000</v>
       </c>
@@ -24430,7 +24438,7 @@
         <v>0.29992854822994475</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>10000</v>
       </c>
@@ -24452,7 +24460,7 @@
         <v>0.27598570964598895</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>10000</v>
       </c>
@@ -24474,7 +24482,7 @@
         <v>0.25378369600519651</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>10000</v>
       </c>
@@ -24496,7 +24504,7 @@
         <v>0.22078596947060733</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>10000</v>
       </c>
@@ -24518,7 +24526,7 @@
         <v>0.18807405001623906</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>15000</v>
       </c>
@@ -24540,7 +24548,7 @@
         <v>0.43951932445599218</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>15000</v>
       </c>
@@ -24562,7 +24570,7 @@
         <v>0.46181227671321862</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>15000</v>
       </c>
@@ -24584,7 +24592,7 @@
         <v>0.4687236115621955</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>15000</v>
       </c>
@@ -24606,7 +24614,7 @@
         <v>0.45909710945112053</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>15000</v>
       </c>
@@ -24628,7 +24636,7 @@
         <v>0.41412146800909383</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>15000</v>
       </c>
@@ -24650,7 +24658,7 @@
         <v>0.36505358882754141</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>15000</v>
       </c>
@@ -24672,7 +24680,7 @@
         <v>0.32854822994478727</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>15000</v>
       </c>
@@ -24694,7 +24702,7 @@
         <v>0.29817473205586226</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>15000</v>
       </c>
@@ -24716,7 +24724,7 @@
         <v>0.27247807729782397</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>15000</v>
       </c>
@@ -24738,7 +24746,7 @@
         <v>0.25144527443975317</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>15000</v>
       </c>
@@ -24760,7 +24768,7 @@
         <v>0.23276388437804482</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>15000</v>
       </c>
@@ -24782,7 +24790,7 @@
         <v>0.21406950308541733</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>15000</v>
       </c>
@@ -24804,7 +24812,7 @@
         <v>0.19595972718415072</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>20000</v>
       </c>
@@ -24826,7 +24834,7 @@
         <v>0.37293926599545307</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>20000</v>
       </c>
@@ -24848,7 +24856,7 @@
         <v>0.3916596297499188</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>20000</v>
       </c>
@@ -24870,7 +24878,7 @@
         <v>0.39805131536213056</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>20000</v>
       </c>
@@ -24892,7 +24900,7 @@
         <v>0.39250405975966224</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>20000</v>
       </c>
@@ -24914,7 +24922,7 @@
         <v>0.35571289379668725</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>20000</v>
       </c>
@@ -24935,8 +24943,11 @@
         <f>D59/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.31481649886326729</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>20000</v>
       </c>
@@ -24957,8 +24968,20 @@
         <f>D60/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.28006495615459565</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H60">
+        <f>C60/(D60*4.44822*316.032*0.001341022*B60*0.85)</f>
+        <v>0.66329642883745499</v>
+      </c>
+      <c r="I60">
+        <f>AVERAGE(H60:H66)</f>
+        <v>0.62330015181572274</v>
+      </c>
+      <c r="J60" s="21">
+        <f>AVERAGE(E54:E66)</f>
+        <v>0.3588425840517489</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>20000</v>
       </c>
@@ -24979,8 +25002,12 @@
         <f>D61/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.255537512179279</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H61">
+        <f t="shared" ref="H61:H66" si="1">C61/(D61*4.44822*316.032*0.001341022*B61*0.85)</f>
+        <v>0.63888301846397089</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>20000</v>
       </c>
@@ -25001,8 +25028,12 @@
         <f>D62/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.23567392010392985</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H62">
+        <f t="shared" si="1"/>
+        <v>0.62187772405796582</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>20000</v>
       </c>
@@ -25023,8 +25054,12 @@
         <f>D63/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.2193179603767457</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H63">
+        <f t="shared" si="1"/>
+        <v>0.61141974961960988</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>20000</v>
       </c>
@@ -25045,8 +25080,12 @@
         <f>D64/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.20618382591750567</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H64">
+        <f t="shared" si="1"/>
+        <v>0.60451967288814845</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>20000</v>
       </c>
@@ -25067,8 +25106,12 @@
         <f>D65/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.19333549853848653</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H65">
+        <f t="shared" si="1"/>
+        <v>0.60644225022579079</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <v>20000</v>
       </c>
@@ -25089,8 +25132,12 @@
         <f>D66/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.18077297823968821</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H66">
+        <f t="shared" si="1"/>
+        <v>0.61666221861711779</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>25000</v>
       </c>
@@ -25104,7 +25151,7 @@
         <v>2421.1</v>
       </c>
       <c r="E67" s="20">
-        <f t="shared" ref="E67:E92" si="1">C67/D67</f>
+        <f t="shared" ref="E67:E92" si="2">C67/D67</f>
         <v>0.26215356656065425</v>
       </c>
       <c r="F67" s="16">
@@ -25112,7 +25159,7 @@
         <v>0.31453069178304643</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>25000</v>
       </c>
@@ -25126,7 +25173,7 @@
         <v>2539.5</v>
       </c>
       <c r="E68" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.24937979917306555</v>
       </c>
       <c r="F68" s="17">
@@ -25134,7 +25181,7 @@
         <v>0.32991230919129588</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>25000</v>
       </c>
@@ -25148,7 +25195,7 @@
         <v>2583</v>
       </c>
       <c r="E69" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.24409601238869533</v>
       </c>
       <c r="F69" s="17">
@@ -25156,7 +25203,7 @@
         <v>0.33556349464111723</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>25000</v>
       </c>
@@ -25170,7 +25217,7 @@
         <v>2560.5</v>
       </c>
       <c r="E70" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.24436633470025387</v>
       </c>
       <c r="F70" s="17">
@@ -25178,7 +25225,7 @@
         <v>0.3326404676843131</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>25000</v>
       </c>
@@ -25192,7 +25239,7 @@
         <v>2328.9</v>
       </c>
       <c r="E71" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26364378032547553</v>
       </c>
       <c r="F71" s="17">
@@ -25200,7 +25247,7 @@
         <v>0.302552776875609</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>25000</v>
       </c>
@@ -25214,7 +25261,7 @@
         <v>2068.1999999999998</v>
       </c>
       <c r="E72" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.29112271540469975</v>
       </c>
       <c r="F72" s="17">
@@ -25222,7 +25269,7 @@
         <v>0.26868463786943808</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>25000</v>
       </c>
@@ -25236,7 +25283,7 @@
         <v>1820.9</v>
       </c>
       <c r="E73" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.31418529298698444</v>
       </c>
       <c r="F73" s="17">
@@ -25244,7 +25291,7 @@
         <v>0.23655732380643066</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>25000</v>
       </c>
@@ -25258,7 +25305,7 @@
         <v>1656.8</v>
       </c>
       <c r="E74" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.35224529212940608</v>
       </c>
       <c r="F74" s="17">
@@ -25266,7 +25313,7 @@
         <v>0.215238713868139</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>25000</v>
       </c>
@@ -25280,7 +25327,7 @@
         <v>1530.9</v>
       </c>
       <c r="E75" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.3925795283819975</v>
       </c>
       <c r="F75" s="17">
@@ -25288,7 +25335,7 @@
         <v>0.19888275414095485</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>25000</v>
       </c>
@@ -25302,7 +25349,7 @@
         <v>1427.5</v>
       </c>
       <c r="E76" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43411558669001754</v>
       </c>
       <c r="F76" s="17">
@@ -25310,7 +25357,7 @@
         <v>0.18544982137057486</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>25000</v>
       </c>
@@ -25324,7 +25371,7 @@
         <v>1344.3</v>
       </c>
       <c r="E77" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.47772074685710042</v>
       </c>
       <c r="F77" s="17">
@@ -25332,7 +25379,7 @@
         <v>0.17464111724585904</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>25000</v>
       </c>
@@ -25346,7 +25393,7 @@
         <v>1272.4000000000001</v>
       </c>
       <c r="E78" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.52499214083621504</v>
       </c>
       <c r="F78" s="17">
@@ -25354,7 +25401,7 @@
         <v>0.16530042221500488</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="9">
         <v>25000</v>
       </c>
@@ -25368,7 +25415,7 @@
         <v>1191.4000000000001</v>
       </c>
       <c r="E79" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.58620110794023828</v>
       </c>
       <c r="F79" s="19">
@@ -25376,7 +25423,7 @@
         <v>0.15477752517050991</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>30000</v>
       </c>
@@ -25390,7 +25437,7 @@
         <v>2025.4</v>
       </c>
       <c r="E80" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.27046509331490071</v>
       </c>
       <c r="F80" s="17">
@@ -25398,7 +25445,7 @@
         <v>0.26312439103605068</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>30000</v>
       </c>
@@ -25412,7 +25459,7 @@
         <v>2122.6</v>
       </c>
       <c r="E81" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25742014510505984</v>
       </c>
       <c r="F81" s="17">
@@ -25420,7 +25467,7 @@
         <v>0.27575186748944464</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>30000</v>
       </c>
@@ -25434,7 +25481,7 @@
         <v>2162.6</v>
       </c>
       <c r="E82" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25150282067881252</v>
       </c>
       <c r="F82" s="17">
@@ -25442,7 +25489,7 @@
         <v>0.28094835985709643</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>30000</v>
       </c>
@@ -25456,7 +25503,7 @@
         <v>2162.6</v>
       </c>
       <c r="E83" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.24965319522796633</v>
       </c>
       <c r="F83" s="17">
@@ -25464,7 +25511,7 @@
         <v>0.28094835985709643</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>30000</v>
       </c>
@@ -25478,7 +25525,7 @@
         <v>1976</v>
       </c>
       <c r="E84" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26776315789473687</v>
       </c>
       <c r="F84" s="17">
@@ -25486,7 +25533,7 @@
         <v>0.25670672296200064</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>30000</v>
       </c>
@@ -25500,7 +25547,7 @@
         <v>1762.4</v>
       </c>
       <c r="E85" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.29334997730367679</v>
       </c>
       <c r="F85" s="17">
@@ -25508,7 +25555,7 @@
         <v>0.22895745371873985</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>30000</v>
       </c>
@@ -25522,7 +25569,7 @@
         <v>1555.6</v>
       </c>
       <c r="E86" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.3111982514785292</v>
       </c>
       <c r="F86" s="17">
@@ -25530,7 +25577,7 @@
         <v>0.20209158817797984</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>30000</v>
       </c>
@@ -25544,7 +25591,7 @@
         <v>1382.5</v>
       </c>
       <c r="E87" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34589511754068714</v>
       </c>
       <c r="F87" s="17">
@@ -25552,7 +25599,7 @@
         <v>0.17960376745696655</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>30000</v>
       </c>
@@ -25566,7 +25613,7 @@
         <v>1276.9000000000001</v>
       </c>
       <c r="E88" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.38640457357663088</v>
       </c>
       <c r="F88" s="17">
@@ -25574,7 +25621,7 @@
         <v>0.16588502760636573</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>30000</v>
       </c>
@@ -25588,7 +25635,7 @@
         <v>1193.7</v>
       </c>
       <c r="E89" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.42665661388958698</v>
       </c>
       <c r="F89" s="17">
@@ -25596,7 +25643,7 @@
         <v>0.1550763234816499</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>30000</v>
       </c>
@@ -25610,7 +25657,7 @@
         <v>1124</v>
       </c>
       <c r="E90" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.46992882562277583</v>
       </c>
       <c r="F90" s="17">
@@ -25618,7 +25665,7 @@
         <v>0.14602143553101657</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>30000</v>
       </c>
@@ -25632,7 +25679,7 @@
         <v>1067.8</v>
       </c>
       <c r="E91" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.51638883686083537</v>
       </c>
       <c r="F91" s="17">
@@ -25640,7 +25687,7 @@
         <v>0.13872036375446573</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="9">
         <v>30000</v>
       </c>
@@ -25654,7 +25701,7 @@
         <v>1002.6</v>
       </c>
       <c r="E92" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.57759824456413322</v>
       </c>
       <c r="F92" s="19">
@@ -25678,14 +25725,14 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -25705,7 +25752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -25727,7 +25774,7 @@
         <v>0.36359857096459891</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>0</v>
       </c>
@@ -25749,7 +25796,7 @@
         <v>0.2564988632672946</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>0</v>
       </c>
@@ -25771,7 +25818,7 @@
         <v>9.7538161740824941E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>0</v>
       </c>
@@ -25793,7 +25840,7 @@
         <v>-0.13083468658655409</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>0</v>
       </c>
@@ -25815,7 +25862,7 @@
         <v>-0.10075998700876908</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>0</v>
       </c>
@@ -25837,7 +25884,7 @@
         <v>-7.972718415069828E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>0</v>
       </c>
@@ -25859,7 +25906,7 @@
         <v>-5.3445924001299119E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>0</v>
       </c>
@@ -25881,7 +25928,7 @@
         <v>-4.9067879181552448E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>0</v>
       </c>
@@ -25903,7 +25950,7 @@
         <v>-5.5199740175381616E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>0</v>
       </c>
@@ -25925,7 +25972,7 @@
         <v>-6.4254628126014943E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>0</v>
       </c>
@@ -25947,7 +25994,7 @@
         <v>-7.8557973367976625E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>0</v>
       </c>
@@ -25969,7 +26016,7 @@
         <v>-9.3458915232218248E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>0</v>
       </c>
@@ -25991,7 +26038,7 @@
         <v>-0.10834686586554076</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>5000</v>
       </c>
@@ -26013,7 +26060,7 @@
         <v>0.31394608639168559</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>5000</v>
       </c>
@@ -26035,7 +26082,7 @@
         <v>0.21973367976615785</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>5000</v>
       </c>
@@ -26057,7 +26104,7 @@
         <v>8.9366677492692434E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5000</v>
       </c>
@@ -26079,7 +26126,7 @@
         <v>-8.8197466709970765E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>5000</v>
       </c>
@@ -26101,7 +26148,7 @@
         <v>-7.2140305293926593E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>5000</v>
       </c>
@@ -26123,7 +26170,7 @@
         <v>-5.6953556349464106E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>5000</v>
       </c>
@@ -26145,7 +26192,7 @@
         <v>-3.4166937317310818E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>5000</v>
       </c>
@@ -26167,7 +26214,7 @@
         <v>-3.4751542708671646E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>5000</v>
       </c>
@@ -26189,7 +26236,7 @@
         <v>-4.0597596622279963E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>5000</v>
       </c>
@@ -26211,7 +26258,7 @@
         <v>-4.9067879181552448E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>5000</v>
       </c>
@@ -26233,7 +26280,7 @@
         <v>-6.1331601169210784E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>5000</v>
       </c>
@@ -26255,7 +26302,7 @@
         <v>-7.5050341019811631E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>5000</v>
       </c>
@@ -26277,7 +26324,7 @@
         <v>-8.8782072101331599E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>10000</v>
       </c>
@@ -26299,7 +26346,7 @@
         <v>0.26955505034101984</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>10000</v>
       </c>
@@ -26321,7 +26368,7 @@
         <v>0.18877557648587204</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>10000</v>
       </c>
@@ -26343,7 +26390,7 @@
         <v>8.1481000324780783E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>10000</v>
       </c>
@@ -26365,7 +26412,7 @@
         <v>-5.9863592075349144E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>10000</v>
       </c>
@@ -26387,7 +26434,7 @@
         <v>-4.9067879181552448E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>10000</v>
       </c>
@@ -26409,7 +26456,7 @@
         <v>-3.8544982137057482E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>10000</v>
       </c>
@@ -26431,7 +26478,7 @@
         <v>-2.073400454693082E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>10000</v>
       </c>
@@ -26453,7 +26500,7 @@
         <v>-2.3657031503734979E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>10000</v>
       </c>
@@ -26475,7 +26522,7 @@
         <v>-2.8619681714842481E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>10000</v>
       </c>
@@ -26497,7 +26544,7 @@
         <v>-3.6505358882754142E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>10000</v>
       </c>
@@ -26519,7 +26566,7 @@
         <v>-4.7314063007469959E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>10000</v>
       </c>
@@ -26541,7 +26588,7 @@
         <v>-5.9577784995128294E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>10000</v>
       </c>
@@ -26563,7 +26610,7 @@
         <v>-7.2140305293926593E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>15000</v>
       </c>
@@ -26585,7 +26632,7 @@
         <v>0.23012666450146152</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>15000</v>
       </c>
@@ -26607,7 +26654,7 @@
         <v>0.16153296524845731</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>15000</v>
       </c>
@@ -26629,7 +26676,7 @@
         <v>7.3595323156869119E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>15000</v>
       </c>
@@ -26651,7 +26698,7 @@
         <v>-3.8843780448197467E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>15000</v>
       </c>
@@ -26673,7 +26720,7 @@
         <v>-3.2997726534589156E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>15000</v>
       </c>
@@ -26695,7 +26742,7 @@
         <v>-2.5995453069178304E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>15000</v>
       </c>
@@ -26717,7 +26764,7 @@
         <v>-1.0509905813575837E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>15000</v>
       </c>
@@ -26739,7 +26786,7 @@
         <v>-1.4602143553101658E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>15000</v>
       </c>
@@ -26761,7 +26808,7 @@
         <v>-1.9278986683988308E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>15000</v>
       </c>
@@ -26783,7 +26830,7 @@
         <v>-2.6580058460539135E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>15000</v>
       </c>
@@ -26805,7 +26852,7 @@
         <v>-3.5634946411172458E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>15000</v>
       </c>
@@ -26827,7 +26874,7 @@
         <v>-4.6430659304969146E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>15000</v>
       </c>
@@ -26849,7 +26896,7 @@
         <v>-5.7823968821045797E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>20000</v>
       </c>
@@ -26871,7 +26918,7 @@
         <v>0.19712893796687236</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>20000</v>
       </c>
@@ -26893,7 +26940,7 @@
         <v>0.13060084443000974</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>20000</v>
       </c>
@@ -26915,7 +26962,7 @@
         <v>6.86326729457616E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>20000</v>
       </c>
@@ -26937,7 +26984,7 @@
         <v>1.1679116596297501E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>20000</v>
       </c>
@@ -26959,7 +27006,7 @@
         <v>8.7560896394933436E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>20000</v>
       </c>
@@ -26981,7 +27028,7 @@
         <v>6.4306593049691455E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>20000</v>
       </c>
@@ -27003,7 +27050,7 @@
         <v>7.5868788567716788E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>20000</v>
       </c>
@@ -27025,7 +27072,7 @@
         <v>5.8460539136083141E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>20000</v>
       </c>
@@ -27047,7 +27094,7 @@
         <v>-7.301071776550829E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>20000</v>
       </c>
@@ -27069,7 +27116,7 @@
         <v>-1.6355959727184153E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>20000</v>
       </c>
@@ -27091,7 +27138,7 @@
         <v>-2.6281260149399157E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>20000</v>
       </c>
@@ -27113,7 +27160,7 @@
         <v>-3.5920753491393308E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <v>20000</v>
       </c>
@@ -27135,7 +27182,7 @@
         <v>-4.6144852224748296E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>25000</v>
       </c>
@@ -27157,7 +27204,7 @@
         <v>0.18544982137057486</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>25000</v>
       </c>
@@ -27179,7 +27226,7 @@
         <v>0.14476128613186098</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>25000</v>
       </c>
@@ -27201,7 +27248,7 @@
         <v>0.10806105878531991</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>25000</v>
       </c>
@@ -27223,7 +27270,7 @@
         <v>7.5634946411172466E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>25000</v>
       </c>
@@ -27245,7 +27292,7 @@
         <v>5.7239363429684963E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>25000</v>
       </c>
@@ -27267,7 +27314,7 @@
         <v>4.4092237739525815E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>25000</v>
       </c>
@@ -27289,7 +27336,7 @@
         <v>3.6219551802533292E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>25000</v>
       </c>
@@ -27311,7 +27358,7 @@
         <v>2.8333874634621628E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>25000</v>
       </c>
@@ -27333,7 +27380,7 @@
         <v>1.9278986683988308E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>25000</v>
       </c>
@@ -27355,7 +27402,7 @@
         <v>8.1714842481325108E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>25000</v>
       </c>
@@ -27377,7 +27424,7 @@
         <v>-2.3384215654433257E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>25000</v>
       </c>
@@ -27399,7 +27446,7 @@
         <v>-1.2848327379019163E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="9">
         <v>25000</v>
       </c>
@@ -27421,7 +27468,7 @@
         <v>-2.4527443975316664E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>30000</v>
       </c>
@@ -27443,7 +27490,7 @@
         <v>0.20239038648911986</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>30000</v>
       </c>
@@ -27465,7 +27512,7 @@
         <v>0.17078272166287756</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>30000</v>
       </c>
@@ -27487,7 +27534,7 @@
         <v>0.14017538161740825</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>30000</v>
       </c>
@@ -27509,7 +27556,7 @@
         <v>0.11068528743098409</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>30000</v>
       </c>
@@ -27531,7 +27578,7 @@
         <v>8.9652484572913291E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>30000</v>
       </c>
@@ -27553,7 +27600,7 @@
         <v>7.4465735628450797E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>30000</v>
       </c>
@@ -27575,7 +27622,7 @@
         <v>5.9577784995128294E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>30000</v>
       </c>
@@ -27597,7 +27644,7 @@
         <v>5.0237089964274111E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>30000</v>
       </c>
@@ -27619,7 +27666,7 @@
         <v>4.1766807405001626E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>30000</v>
       </c>
@@ -27641,7 +27688,7 @@
         <v>3.1542708671646637E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>30000</v>
       </c>
@@ -27663,7 +27710,7 @@
         <v>2.1032802858070802E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>30000</v>
       </c>
@@ -27685,7 +27732,7 @@
         <v>1.0224098733354985E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="9">
         <v>30000</v>
       </c>

</xml_diff>

<commit_message>
Major modifications to OperatingConditions and PowerPlant. Some errors have still to be fixed.
</commit_message>
<xml_diff>
--- a/DOCS/TurboporpEngineModel/PW2750.xlsx
+++ b/DOCS/TurboporpEngineModel/PW2750.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr codeName="Questa_cartella_di_lavoro"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\JPAD\jpad\DOCS\TurboporpEngineModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JPAD\jpad\DOCS\TurboporpEngineModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CA0E64-C443-4530-972F-CC00DC0D680E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PW2750 TAKE-OFF" sheetId="1" r:id="rId1"/>
@@ -18,17 +19,22 @@
     <sheet name="PW2750 CRUISE" sheetId="4" r:id="rId4"/>
     <sheet name="PW2750 IDLE" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
   <si>
     <t>Altitude</t>
   </si>
@@ -50,11 +56,20 @@
   <si>
     <t>MEAN</t>
   </si>
+  <si>
+    <t>Power (hp)</t>
+  </si>
+  <si>
+    <t>SFC (lb/hp*hr)</t>
+  </si>
+  <si>
+    <t>Power (W)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -263,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -296,6 +311,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -18352,11 +18371,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -19543,7 +19562,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:F92"/>
   <sheetViews>
@@ -21588,11 +21607,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Foglio3"/>
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
@@ -23633,12 +23652,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Foglio4"/>
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23646,6 +23665,9 @@
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -24350,7 +24372,7 @@
         <v>0.46668398830789221</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>10000</v>
       </c>
@@ -24372,7 +24394,7 @@
         <v>0.41061383566092885</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>10000</v>
       </c>
@@ -24394,7 +24416,7 @@
         <v>0.36650860669048391</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>10000</v>
       </c>
@@ -24415,18 +24437,27 @@
         <f>D35/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.32941864241636892</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="22">
         <v>10000</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="23">
         <v>0.4</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="23">
         <v>960.5</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="24">
         <v>2308.6999999999998</v>
       </c>
       <c r="E36" s="15">
@@ -24437,8 +24468,20 @@
         <f>D36/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.29992854822994475</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I36" s="25">
+        <f>B36*322.269*D36*4.44822</f>
+        <v>1323830.1997565064</v>
+      </c>
+      <c r="J36" s="25">
+        <f>I36*0.00134102</f>
+        <v>1775.2827744774702</v>
+      </c>
+      <c r="K36" s="25">
+        <f>C36/J36</f>
+        <v>0.54104056762602781</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>10000</v>
       </c>
@@ -24460,7 +24503,7 @@
         <v>0.27598570964598895</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>10000</v>
       </c>
@@ -24482,7 +24525,7 @@
         <v>0.25378369600519651</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>10000</v>
       </c>
@@ -24504,7 +24547,7 @@
         <v>0.22078596947060733</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>10000</v>
       </c>
@@ -24526,7 +24569,7 @@
         <v>0.18807405001623906</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>15000</v>
       </c>
@@ -24548,7 +24591,7 @@
         <v>0.43951932445599218</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>15000</v>
       </c>
@@ -24570,7 +24613,7 @@
         <v>0.46181227671321862</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>15000</v>
       </c>
@@ -24592,7 +24635,7 @@
         <v>0.4687236115621955</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>15000</v>
       </c>
@@ -24614,7 +24657,7 @@
         <v>0.45909710945112053</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>15000</v>
       </c>
@@ -24636,7 +24679,7 @@
         <v>0.41412146800909383</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>15000</v>
       </c>
@@ -24658,7 +24701,7 @@
         <v>0.36505358882754141</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>15000</v>
       </c>
@@ -24680,7 +24723,7 @@
         <v>0.32854822994478727</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>15000</v>
       </c>
@@ -24701,30 +24744,51 @@
         <f>D48/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.29817473205586226</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="8">
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22">
         <v>15000</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="23">
         <v>0.4</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="23">
         <v>849.7</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="24">
         <v>2097.4</v>
       </c>
       <c r="E49" s="15">
-        <f t="shared" si="0"/>
+        <f>C49/D49</f>
         <v>0.4051206255363784</v>
       </c>
       <c r="F49" s="17">
         <f>D49/'PW2750 TAKE-OFF'!$D$2</f>
         <v>0.27247807729782397</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="25">
+        <f>B49*322.269*D49*4.44822</f>
+        <v>1202668.8010435728</v>
+      </c>
+      <c r="J49" s="25">
+        <f>I49*0.00134102</f>
+        <v>1612.8029155754521</v>
+      </c>
+      <c r="K49" s="25">
+        <f>C49/J49</f>
+        <v>0.52684676583488499</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>15000</v>
       </c>
@@ -24746,7 +24810,7 @@
         <v>0.25144527443975317</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>15000</v>
       </c>
@@ -24768,7 +24832,7 @@
         <v>0.23276388437804482</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>15000</v>
       </c>
@@ -24790,7 +24854,7 @@
         <v>0.21406950308541733</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>15000</v>
       </c>
@@ -24812,7 +24876,7 @@
         <v>0.19595972718415072</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>20000</v>
       </c>
@@ -24834,7 +24898,7 @@
         <v>0.37293926599545307</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>20000</v>
       </c>
@@ -24856,7 +24920,7 @@
         <v>0.3916596297499188</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>20000</v>
       </c>
@@ -24878,7 +24942,7 @@
         <v>0.39805131536213056</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>20000</v>
       </c>
@@ -24900,7 +24964,7 @@
         <v>0.39250405975966224</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>20000</v>
       </c>
@@ -24922,7 +24986,7 @@
         <v>0.35571289379668725</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>20000</v>
       </c>
@@ -24947,7 +25011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>20000</v>
       </c>
@@ -24981,7 +25045,7 @@
         <v>0.3588425840517489</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>20000</v>
       </c>
@@ -25007,7 +25071,7 @@
         <v>0.63888301846397089</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>20000</v>
       </c>
@@ -25033,7 +25097,7 @@
         <v>0.62187772405796582</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>20000</v>
       </c>
@@ -25059,7 +25123,7 @@
         <v>0.61141974961960988</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>20000</v>
       </c>
@@ -25711,13 +25775,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Foglio5"/>
   <dimension ref="A1:F92"/>
   <sheetViews>

</xml_diff>